<commit_message>
Calculate deaths at each step, add kid parameters
</commit_message>
<xml_diff>
--- a/0 - Parameters/Mixing_15_mar_2020.xlsx
+++ b/0 - Parameters/Mixing_15_mar_2020.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abilinski/Dropbox/COVID19/0 - Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB742EF-631B-684E-921D-67E317F4CC6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A60C8EE-D4BE-2947-A2B6-B5AA4CC2C8B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21140" xr2:uid="{139E60A7-A13C-2640-9DF0-C4936CA4B7DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A15" sqref="A15:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,78 +504,78 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.26097125345400002</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.115155067298</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2.5716837201400001E-3</v>
+      <c r="B2">
+        <v>9.761902954</v>
+      </c>
+      <c r="C2">
+        <v>2.2706403989999999</v>
+      </c>
+      <c r="D2">
+        <v>0.29226176269999998</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G2">
         <f>B2</f>
-        <v>0.26097125345400002</v>
+        <v>9.761902954</v>
       </c>
       <c r="H2">
         <f>B2*B7</f>
-        <v>0.17467722002775843</v>
+        <v>6.5339842899058853</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.14324153902100001</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.43960213421400002</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5.2637081386900002E-3</v>
+      <c r="B3">
+        <v>6.6876464320000002</v>
+      </c>
+      <c r="C3">
+        <v>10.333415990000001</v>
+      </c>
+      <c r="D3">
+        <v>0.88528063099999998</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
       <c r="G3">
         <f>C2</f>
-        <v>0.115155067298</v>
+        <v>2.2706403989999999</v>
       </c>
       <c r="H3">
         <f>C2*C7</f>
-        <v>0.12213795542388343</v>
+        <v>2.4083297621549611</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
-        <v>1.09536535559E-2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2.3325545953100001E-2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>5.1987854322499997E-3</v>
+      <c r="B4">
+        <v>0.91568368420000001</v>
+      </c>
+      <c r="C4">
+        <v>1.01411684</v>
+      </c>
+      <c r="D4">
+        <v>1.2494830159999999</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4">
         <f>D2</f>
-        <v>2.5716837201400001E-3</v>
+        <v>0.29226176269999998</v>
       </c>
       <c r="H4">
         <f>D2*D7</f>
-        <v>4.5502034468622686E-3</v>
+        <v>0.5171127653097195</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -588,11 +588,11 @@
       </c>
       <c r="G5">
         <f>B3</f>
-        <v>0.14324153902100001</v>
+        <v>6.6876464320000002</v>
       </c>
       <c r="H5">
         <f>B3*B8</f>
-        <v>0.16255618517012993</v>
+        <v>7.5894066705969498</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -613,11 +613,11 @@
       </c>
       <c r="G6">
         <f>C3</f>
-        <v>0.43960213421400002</v>
+        <v>10.333415990000001</v>
       </c>
       <c r="H6">
         <f>C3*C8</f>
-        <v>0.49109185299021735</v>
+        <v>11.543748338076719</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -638,11 +638,11 @@
       </c>
       <c r="G7">
         <f>D3</f>
-        <v>5.2637081386900002E-3</v>
+        <v>0.88528063099999998</v>
       </c>
       <c r="H7">
         <f>D3*D8</f>
-        <v>6.8483211553019311E-3</v>
+        <v>1.151789938559395</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -663,11 +663,11 @@
       </c>
       <c r="G8">
         <f>B4</f>
-        <v>1.09536535559E-2</v>
+        <v>0.91568368420000001</v>
       </c>
       <c r="H8">
         <f>B4*B9</f>
-        <v>1.8765792699775748E-2</v>
+        <v>1.5687487383612295</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -688,11 +688,11 @@
       </c>
       <c r="G9">
         <f>C4</f>
-        <v>2.3325545953100001E-2</v>
+        <v>1.01411684</v>
       </c>
       <c r="H9">
         <f>C4*C9</f>
-        <v>3.3294137875984439E-2</v>
+        <v>1.44751792567712</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -701,11 +701,11 @@
       </c>
       <c r="G10">
         <f>D4</f>
-        <v>5.1987854322499997E-3</v>
+        <v>1.2494830159999999</v>
       </c>
       <c r="H10">
         <f>D4*D9</f>
-        <v>5.9318557684807077E-3</v>
+        <v>1.4256701171201278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pull together calibration and make graphs
</commit_message>
<xml_diff>
--- a/0 - Parameters/Mixing_15_mar_2020.xlsx
+++ b/0 - Parameters/Mixing_15_mar_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abilinski/Dropbox/COVID19/0 - Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A60C8EE-D4BE-2947-A2B6-B5AA4CC2C8B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5848FFB-6873-2D48-91C1-EA5EB164B541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21140" xr2:uid="{139E60A7-A13C-2640-9DF0-C4936CA4B7DC}"/>
+    <workbookView xWindow="-26720" yWindow="-1460" windowWidth="38400" windowHeight="21140" xr2:uid="{139E60A7-A13C-2640-9DF0-C4936CA4B7DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E20"/>
+      <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +525,7 @@
       </c>
       <c r="H2">
         <f>B2*B7</f>
-        <v>6.5339842899058853</v>
+        <v>7.1729447668084791</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -550,7 +550,7 @@
       </c>
       <c r="H3">
         <f>C2*C7</f>
-        <v>2.4083297621549611</v>
+        <v>2.3740975874996368</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -575,7 +575,7 @@
       </c>
       <c r="H4">
         <f>D2*D7</f>
-        <v>0.5171127653097195</v>
+        <v>0.4302569533617201</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -592,7 +592,7 @@
       </c>
       <c r="H5">
         <f>B3*B8</f>
-        <v>7.5894066705969498</v>
+        <v>7.3321188683004035</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -617,21 +617,21 @@
       </c>
       <c r="H6">
         <f>C3*C8</f>
-        <v>11.543748338076719</v>
+        <v>11.20096826285644</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1">
-        <v>0.66933509999999996</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.0606390000000001</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.7693479999999999</v>
+      <c r="B7">
+        <v>0.73478960000000004</v>
+      </c>
+      <c r="C7">
+        <v>1.045563</v>
+      </c>
+      <c r="D7">
+        <v>1.4721630000000001</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -642,21 +642,21 @@
       </c>
       <c r="H7">
         <f>D3*D8</f>
-        <v>1.151789938559395</v>
+        <v>1.069243716683062</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1">
-        <v>1.1348396999999999</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.1171279999999999</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.301045</v>
+      <c r="B8">
+        <v>1.0963676</v>
+      </c>
+      <c r="C8">
+        <v>1.0839559999999999</v>
+      </c>
+      <c r="D8">
+        <v>1.207802</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -667,21 +667,21 @@
       </c>
       <c r="H8">
         <f>B4*B9</f>
-        <v>1.5687487383612295</v>
+        <v>1.3315228410006408</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1">
-        <v>1.7131993999999999</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.427368</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.141008</v>
+      <c r="B9">
+        <v>1.4541297</v>
+      </c>
+      <c r="C9">
+        <v>1.2884869999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.0999989999999999</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="H9">
         <f>C4*C9</f>
-        <v>1.44751792567712</v>
+        <v>1.30667636482108</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -705,7 +705,7 @@
       </c>
       <c r="H10">
         <f>D4*D9</f>
-        <v>1.4256701171201278</v>
+        <v>1.3744300681169839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>